<commit_message>
Add Customer Environment to Playbook
Update the Playbook to include the Customer Environment name (helpful
for better identification of where metrics originated from).
</commit_message>
<xml_diff>
--- a/python--deployment-metric-parser/examples/Playbook_1_Sample.xlsx
+++ b/python--deployment-metric-parser/examples/Playbook_1_Sample.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-31540" yWindow="460" windowWidth="30180" windowHeight="11220" tabRatio="500"/>
+    <workbookView xWindow="-33500" yWindow="460" windowWidth="30180" windowHeight="11220" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="2" r:id="rId1"/>
+    <sheet name="Playbook" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
   <si>
     <t>Step</t>
   </si>
@@ -186,6 +187,33 @@
   </si>
   <si>
     <t>This did not go well</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Upgrade Date</t>
+  </si>
+  <si>
+    <t>Upgrade Start Time</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Red SW, Blue Component, Green 3rd Party</t>
+  </si>
+  <si>
+    <t>11:00AM</t>
+  </si>
+  <si>
+    <t>Customer A</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>UAT</t>
   </si>
 </sst>
 </file>
@@ -235,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -262,6 +290,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,11 +571,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="56.33203125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="10">
+        <v>43105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Update Playbook Parser for Installer and Lead
Update the playbook parser to include fields for the installer version
and lead installer.
</commit_message>
<xml_diff>
--- a/python--deployment-metric-parser/examples/Playbook_1_Sample.xlsx
+++ b/python--deployment-metric-parser/examples/Playbook_1_Sample.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33500" yWindow="460" windowWidth="30180" windowHeight="11220" tabRatio="500"/>
+    <workbookView xWindow="-32880" yWindow="460" windowWidth="19140" windowHeight="14540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
     <sheet name="Playbook" sheetId="1" r:id="rId2"/>
+    <sheet name="Task States" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
   <si>
     <t>Step</t>
   </si>
@@ -214,6 +215,27 @@
   </si>
   <si>
     <t>UAT</t>
+  </si>
+  <si>
+    <t>Installer Version</t>
+  </si>
+  <si>
+    <t>18.0.1</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Blocked</t>
+  </si>
+  <si>
+    <t>Joe Schmoe</t>
+  </si>
+  <si>
+    <t>Lead</t>
   </si>
 </sst>
 </file>
@@ -571,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,6 +645,22 @@
         <v>57</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -632,7 +670,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -982,5 +1023,50 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Task States'!$A$1:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G1000</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update to Gather Total Metrics
Update the Playbook gatherer to collect metrics about every single
deployment for every customer/environment in a single dictionary for
better future aggregation.
</commit_message>
<xml_diff>
--- a/python--deployment-metric-parser/examples/Playbook_1_Sample.xlsx
+++ b/python--deployment-metric-parser/examples/Playbook_1_Sample.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-32880" yWindow="460" windowWidth="19140" windowHeight="14540" tabRatio="500"/>
+    <workbookView xWindow="-33360" yWindow="460" windowWidth="33000" windowHeight="14540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="86">
   <si>
     <t>Step</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Actual End Time</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -199,12 +196,6 @@
     <t>Upgrade Start Time</t>
   </si>
   <si>
-    <t>Software</t>
-  </si>
-  <si>
-    <t>Red SW, Blue Component, Green 3rd Party</t>
-  </si>
-  <si>
     <t>11:00AM</t>
   </si>
   <si>
@@ -214,9 +205,6 @@
     <t>Environment</t>
   </si>
   <si>
-    <t>UAT</t>
-  </si>
-  <si>
     <t>Installer Version</t>
   </si>
   <si>
@@ -236,6 +224,70 @@
   </si>
   <si>
     <t>Lead</t>
+  </si>
+  <si>
+    <t>Errors</t>
+  </si>
+  <si>
+    <t>Additional Notes</t>
+  </si>
+  <si>
+    <t>PRODUCT</t>
+  </si>
+  <si>
+    <t>INCLUDED?</t>
+  </si>
+  <si>
+    <t>SOURCE VERSION</t>
+  </si>
+  <si>
+    <t>TARGET VERSION</t>
+  </si>
+  <si>
+    <t>Actual Duration
+(Minutes)</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>5.6.1</t>
+  </si>
+  <si>
+    <t>6.1.3</t>
+  </si>
+  <si>
+    <t>6.4.2</t>
+  </si>
+  <si>
+    <t>5.2.2</t>
+  </si>
+  <si>
+    <t>7.8.1</t>
+  </si>
+  <si>
+    <t>A_SW</t>
+  </si>
+  <si>
+    <t>B_SW</t>
+  </si>
+  <si>
+    <t>C_SW</t>
+  </si>
+  <si>
+    <t>D_SW</t>
+  </si>
+  <si>
+    <t>E_SW</t>
+  </si>
+  <si>
+    <t>SIT</t>
+  </si>
+  <si>
+    <t>Some note</t>
+  </si>
+  <si>
+    <t>Another note</t>
   </si>
 </sst>
 </file>
@@ -285,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -316,6 +368,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,73 +651,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="56.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="B3" s="10">
         <v>43105</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>56</v>
-      </c>
       <c r="B5" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>67</v>
-      </c>
+      <c r="C8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="11"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -668,11 +795,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -682,17 +809,19 @@
     <col min="4" max="4" width="18.5" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="17.5" style="5" customWidth="1"/>
-    <col min="8" max="8" width="15.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="63.1640625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="22" style="5" customWidth="1"/>
+    <col min="11" max="11" width="38.6640625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -704,10 +833,10 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>4</v>
@@ -715,311 +844,399 @@
       <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="6">
         <v>0.46875</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="J2" s="5">
+        <v>30</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="6">
         <v>0.46875</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0.48958333333333331</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="5">
+        <v>15</v>
+      </c>
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J4" s="5">
+        <v>30</v>
+      </c>
+      <c r="L4" s="9"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="3">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="F5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+      <c r="J5" s="5">
+        <v>72</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="3">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="6">
         <v>0.55208333333333337</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="6">
         <v>0.56041666666666667</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="J6" s="5">
+        <v>48</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>39</v>
-      </c>
       <c r="F7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J7" s="5">
+        <v>70</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="F8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J8" s="5">
+        <v>516</v>
+      </c>
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="3">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9" s="6">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J9" s="5">
+        <v>44</v>
+      </c>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="3">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D10" s="6">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="H10" s="6">
         <v>3.125E-2</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="J10" s="5">
+        <v>62</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3">
         <v>10</v>
       </c>
       <c r="C11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="F11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>51</v>
-      </c>
+      <c r="J11" s="5">
+        <v>8</v>
+      </c>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L20" s="9"/>
+    </row>
+    <row r="21" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L23" s="9"/>
+    </row>
+    <row r="24" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L24" s="9"/>
+    </row>
+    <row r="25" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L25" s="9"/>
+    </row>
+    <row r="26" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L26" s="9"/>
+    </row>
+    <row r="27" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L27" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1048,22 +1265,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>